<commit_message>
Correcting displacement test point
</commit_message>
<xml_diff>
--- a/10-2testpoint_displacement.xlsx
+++ b/10-2testpoint_displacement.xlsx
@@ -27,12 +27,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>y</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>ecc</t>
   </si>
 </sst>
 </file>
@@ -347,564 +350,839 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-3.4</v>
       </c>
       <c r="B2">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <f>IF(ABS(A2)&gt;=ABS(B2),ABS(A2),ABS(B2))</f>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3.4</v>
       </c>
       <c r="B3">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <f t="shared" ref="C3:C66" si="0">IF(ABS(A3)&gt;=ABS(B3),ABS(A3),ABS(B3))</f>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-5</v>
       </c>
       <c r="B4">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-5.6</v>
       </c>
       <c r="B5">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-3.4</v>
       </c>
       <c r="B6">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3.4</v>
       </c>
       <c r="B7">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5.6</v>
       </c>
       <c r="B8">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>-5</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>-5.6</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>-3.4</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3.4</v>
       </c>
       <c r="B14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.6</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8.3000000000000007</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B18">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>-5</v>
       </c>
       <c r="B19">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>-5.6</v>
       </c>
       <c r="B20">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>-3.4</v>
       </c>
       <c r="B21">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3.4</v>
       </c>
       <c r="B22">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5.6</v>
       </c>
       <c r="B23">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
       <c r="B24">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8.3000000000000007</v>
       </c>
       <c r="B25">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-9.6999999999999993</v>
       </c>
       <c r="B26">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B27">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>-5</v>
       </c>
       <c r="B28">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>-5.6</v>
       </c>
       <c r="B29">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-3.4</v>
       </c>
       <c r="B30">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3.4</v>
       </c>
       <c r="B31">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>5.6</v>
       </c>
       <c r="B32">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8.3000000000000007</v>
       </c>
       <c r="B34">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>9.6999999999999993</v>
       </c>
       <c r="B35">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-9.6999999999999993</v>
       </c>
       <c r="B36">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B37">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-5</v>
       </c>
       <c r="B38">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-5.6</v>
       </c>
       <c r="B39">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-3.4</v>
       </c>
       <c r="B40">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3.4</v>
       </c>
       <c r="B41">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5.6</v>
       </c>
       <c r="B42">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
       <c r="B43">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>8.3000000000000007</v>
       </c>
       <c r="B44">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>9.6999999999999993</v>
       </c>
       <c r="B45">
         <v>-3.4</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B46">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-5</v>
       </c>
       <c r="B47">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-5.6</v>
       </c>
       <c r="B48">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-3.4</v>
       </c>
       <c r="B49">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3.4</v>
       </c>
       <c r="B50">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>5.6</v>
       </c>
       <c r="B51">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>5</v>
       </c>
       <c r="B52">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>8.3000000000000007</v>
       </c>
       <c r="B53">
         <v>-5.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-8.3000000000000007</v>
       </c>
       <c r="B54">
         <v>-5</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-5</v>
       </c>
       <c r="B55">
         <v>-5</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-5.6</v>
       </c>
       <c r="B56">
         <v>-5</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-3.4</v>
       </c>
       <c r="B57">
         <v>-5</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3.4</v>
       </c>
       <c r="B58">
         <v>-5</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>5.6</v>
       </c>
       <c r="B59">
         <v>-5</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>5</v>
       </c>
       <c r="B60">
         <v>-5</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>8.3000000000000007</v>
       </c>
       <c r="B61">
         <v>-5</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-5</v>
       </c>
       <c r="B62">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-5.6</v>
       </c>
       <c r="B63">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-3.4</v>
       </c>
       <c r="B64">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3.4</v>
       </c>
       <c r="B65">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>5.6</v>
       </c>
       <c r="B66">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>5</v>
       </c>
       <c r="B67">
         <v>-8.3000000000000007</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <f t="shared" ref="C67:C69" si="1">IF(ABS(A67)&gt;=ABS(B67),ABS(A67),ABS(B67))</f>
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-3.4</v>
       </c>
       <c r="B68">
         <v>-9.6999999999999993</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>3.4</v>
       </c>
       <c r="B69">
         <v>-9.6999999999999993</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>9.6999999999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>